<commit_message>
excel logic & add hsot
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -10,13 +10,19 @@
     <sheet name="General data" sheetId="1" r:id="rId1"/>
     <sheet name="Consistent Error Baseline" sheetId="2" r:id="rId2"/>
     <sheet name="Consistent Error XAI" sheetId="3" r:id="rId3"/>
+    <sheet name="Consistent Error Baseline-NoTP" sheetId="4" r:id="rId4"/>
+    <sheet name="Consistent Error Baseline-TP" sheetId="5" r:id="rId5"/>
+    <sheet name="Consistent Error XAI-NoTP" sheetId="6" r:id="rId6"/>
+    <sheet name="Consistent Error XAI-TP" sheetId="7" r:id="rId7"/>
+    <sheet name="JAS" sheetId="8" r:id="rId8"/>
+    <sheet name="Consistent Error AI" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="125">
   <si>
     <t>ID</t>
   </si>
@@ -105,36 +111,39 @@
     <t>&lt;5 years</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>completed</t>
-  </si>
-  <si>
-    <t>kk</t>
-  </si>
-  <si>
-    <t>ll</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>open</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>test@bla.de</t>
   </si>
   <si>
@@ -153,25 +162,43 @@
     <t>10,11,12,13,14,15,16,17,18,20,21,22,23,24,25,26,27,28</t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>&gt;15 years</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>jony.ive@apple.com</t>
+  </si>
+  <si>
+    <t>11,12,13,14,15,16,17,18,10,21,22,23,24,25,26,27,28,20</t>
+  </si>
+  <si>
     <t>Prefer not to say</t>
   </si>
   <si>
     <t>&gt;55</t>
   </si>
   <si>
-    <t>&gt;15 years</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>jony.ive@apple.com</t>
-  </si>
-  <si>
-    <t>11,12,13,14,15,16,17,18,10,21,22,23,24,25,26,27,28,20</t>
+    <t>33</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>54</t>
   </si>
   <si>
     <t>slide1</t>
@@ -234,76 +261,142 @@
     <t>label</t>
   </si>
   <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>overestimation</t>
+  </si>
+  <si>
+    <t>no tendency</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>underestimation</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>78</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
-    <t>3232</t>
-  </si>
-  <si>
-    <t>qw</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>59</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>74</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t>80%</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>50</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>AI-underestimation</t>
+  </si>
+  <si>
+    <t>AI-no-deviation</t>
+  </si>
+  <si>
+    <t>AI-overestimation</t>
   </si>
 </sst>
 </file>
@@ -785,13 +878,13 @@
         <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P3" t="s">
         <v>30</v>
@@ -800,82 +893,247 @@
         <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="T3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="V3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="W3" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="X3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:31">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L5" t="s">
         <v>49</v>
       </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" t="s">
+        <v>50</v>
+      </c>
+      <c r="W5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V6" t="s">
+        <v>58</v>
+      </c>
+      <c r="W6" t="s">
+        <v>39</v>
+      </c>
+      <c r="X6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -896,64 +1154,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="L1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="N1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="O1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="Q1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="R1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="S1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="T1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="U1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -961,103 +1219,205 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="O2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="P2" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="Q2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R2" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="S2" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="T2">
+        <v>11.77777777777778</v>
+      </c>
+      <c r="U2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" t="s">
+        <v>94</v>
+      </c>
+      <c r="S4" t="s">
         <v>87</v>
       </c>
-      <c r="H4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K4" t="s">
-        <v>91</v>
+      <c r="T4">
+        <v>-8.166666666666666</v>
+      </c>
+      <c r="U4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" t="s">
+        <v>92</v>
+      </c>
+      <c r="O5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P5" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>108</v>
+      </c>
+      <c r="R5" t="s">
+        <v>101</v>
+      </c>
+      <c r="S5" t="s">
+        <v>83</v>
+      </c>
+      <c r="T5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="U5" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1078,64 +1438,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="L1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="N1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="O1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="P1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="Q1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="R1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="S1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="T1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="U1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1143,58 +1503,1033 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" t="s">
         <v>94</v>
       </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L2" t="s">
-        <v>92</v>
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2">
+        <v>22.5</v>
+      </c>
+      <c r="U2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" t="s">
+        <v>94</v>
+      </c>
+      <c r="S4" t="s">
+        <v>104</v>
+      </c>
+      <c r="T4">
+        <v>-11.88888888888889</v>
+      </c>
+      <c r="U4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s">
         <v>50</v>
       </c>
+      <c r="I5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O5" t="s">
+        <v>107</v>
+      </c>
+      <c r="P5" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>118</v>
+      </c>
+      <c r="R5" t="s">
+        <v>120</v>
+      </c>
+      <c r="S5" t="s">
+        <v>121</v>
+      </c>
+      <c r="T5">
+        <v>6.555555555555555</v>
+      </c>
+      <c r="U5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2">
+        <v>14.55555555555556</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4">
+        <v>-5.777777777777778</v>
+      </c>
+      <c r="L4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
       <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="L5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4">
+        <v>-10.55555555555556</v>
+      </c>
+      <c r="L4" t="s">
         <v>95</v>
       </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="L5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>26.22222222222222</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4">
+        <v>-10.66666666666667</v>
+      </c>
+      <c r="L4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="L5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>18.77777777777778</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4">
+        <v>-13.11111111111111</v>
+      </c>
+      <c r="L4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5">
+        <v>7.444444444444445</v>
+      </c>
+      <c r="L5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>0.2062648602826659</v>
+      </c>
+      <c r="C2">
+        <v>0.3421811079011891</v>
+      </c>
+      <c r="D2">
+        <v>0.4515158771624289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>0.4895634275500794</v>
+      </c>
+      <c r="C4">
+        <v>0.06481481481481481</v>
+      </c>
+      <c r="D4">
+        <v>0.01472962066182405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>0.9081529581529582</v>
+      </c>
+      <c r="C5">
+        <v>0.8650793650793651</v>
+      </c>
+      <c r="D5">
+        <v>0.926440329218107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>15.33333333333333</v>
+      </c>
+      <c r="C2">
+        <v>19.83333333333333</v>
+      </c>
+      <c r="D2">
+        <v>32.33333333333334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>-18.5</v>
+      </c>
+      <c r="C4">
+        <v>-11.66666666666667</v>
+      </c>
+      <c r="D4">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>-16.33333333333333</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix early slide switch
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="142">
   <si>
     <t>ID</t>
   </si>
@@ -201,6 +201,27 @@
     <t>54</t>
   </si>
   <si>
+    <t>joluga@web.de</t>
+  </si>
+  <si>
+    <t>12,13,14,15,16,17,18,10,11,22,23,24,25,26,27,28,20,21</t>
+  </si>
+  <si>
+    <t>5-10 years</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
     <t>slide1</t>
   </si>
   <si>
@@ -279,9 +300,6 @@
     <t>75</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
@@ -321,9 +339,6 @@
     <t>66</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -369,6 +384,18 @@
     <t>57</t>
   </si>
   <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
     <t>69</t>
   </si>
   <si>
@@ -396,9 +423,6 @@
     <t>64</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>42</t>
   </si>
   <si>
@@ -412,6 +436,9 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
   <si>
     <t>AI-underestimation</t>
@@ -752,7 +779,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1160,6 +1187,101 @@
         <v>36</v>
       </c>
     </row>
+    <row r="7" spans="1:31">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" t="s">
+        <v>30</v>
+      </c>
+      <c r="V7" t="s">
+        <v>64</v>
+      </c>
+      <c r="W7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1167,7 +1289,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1178,64 +1300,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="L1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="M1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="N1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="P1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="Q1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="R1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="S1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="T1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="U1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1243,64 +1365,64 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="M2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="N2" t="s">
         <v>37</v>
       </c>
       <c r="O2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="P2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="Q2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="R2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="S2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="T2">
         <v>7.944444444444445</v>
       </c>
       <c r="U2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1311,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="U3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1319,34 +1441,34 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="L4" t="s">
         <v>49</v>
@@ -1355,19 +1477,19 @@
         <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="O4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="P4" t="s">
         <v>57</v>
       </c>
       <c r="Q4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="S4" t="s">
         <v>38</v>
@@ -1376,7 +1498,7 @@
         <v>-8.166666666666666</v>
       </c>
       <c r="U4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1384,64 +1506,129 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="J5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
         <v>37</v>
       </c>
       <c r="M5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="N5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="O5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P5" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="Q5" t="s">
+        <v>119</v>
+      </c>
+      <c r="R5" t="s">
         <v>114</v>
       </c>
-      <c r="R5" t="s">
-        <v>109</v>
-      </c>
       <c r="S5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="T5">
         <v>0.3888888888888889</v>
       </c>
       <c r="U5" t="s">
-        <v>96</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" t="s">
+        <v>112</v>
+      </c>
+      <c r="O6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P6" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>112</v>
+      </c>
+      <c r="R6" t="s">
+        <v>123</v>
+      </c>
+      <c r="S6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T6">
+        <v>-12.38888888888889</v>
+      </c>
+      <c r="U6" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1638,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1462,64 +1649,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="L1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="M1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="N1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="P1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="Q1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="R1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="S1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="T1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="U1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1527,64 +1714,64 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="L2" t="s">
         <v>49</v>
       </c>
       <c r="M2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="N2" t="s">
+        <v>131</v>
+      </c>
+      <c r="O2" t="s">
+        <v>91</v>
+      </c>
+      <c r="P2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>132</v>
+      </c>
+      <c r="R2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S2" t="s">
         <v>122</v>
-      </c>
-      <c r="O2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>123</v>
-      </c>
-      <c r="R2" t="s">
-        <v>94</v>
-      </c>
-      <c r="S2" t="s">
-        <v>124</v>
       </c>
       <c r="T2">
         <v>16.61111111111111</v>
       </c>
       <c r="U2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1595,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="U3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1603,55 +1790,55 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
         <v>49</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="M4" t="s">
         <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="O4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="S4" t="s">
         <v>37</v>
@@ -1660,7 +1847,7 @@
         <v>-11.88888888888889</v>
       </c>
       <c r="U4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1668,64 +1855,105 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
         <v>49</v>
       </c>
       <c r="I5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" t="s">
+        <v>136</v>
+      </c>
+      <c r="M5" t="s">
         <v>127</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
+        <v>95</v>
+      </c>
+      <c r="O5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>127</v>
+      </c>
+      <c r="R5" t="s">
         <v>97</v>
       </c>
-      <c r="K5" t="s">
-        <v>124</v>
-      </c>
-      <c r="L5" t="s">
-        <v>128</v>
-      </c>
-      <c r="M5" t="s">
-        <v>118</v>
-      </c>
-      <c r="N5" t="s">
-        <v>89</v>
-      </c>
-      <c r="O5" t="s">
-        <v>113</v>
-      </c>
-      <c r="P5" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>118</v>
-      </c>
-      <c r="R5" t="s">
-        <v>91</v>
-      </c>
       <c r="S5" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="T5">
         <v>6.555555555555555</v>
       </c>
       <c r="U5" t="s">
-        <v>95</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" t="s">
+        <v>106</v>
+      </c>
+      <c r="T6">
+        <v>-14.66666666666667</v>
+      </c>
+      <c r="U6" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1735,7 +1963,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1746,37 +1974,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1784,37 +2012,37 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>11</v>
       </c>
       <c r="L2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1827,7 +2055,7 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
@@ -1836,19 +2064,19 @@
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
         <v>38</v>
@@ -1857,7 +2085,7 @@
         <v>-5.777777777777778</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1865,37 +2093,75 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="H5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" t="s">
         <v>114</v>
       </c>
-      <c r="I5" t="s">
-        <v>109</v>
-      </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="K5">
         <v>0.4444444444444444</v>
       </c>
       <c r="L5" t="s">
-        <v>96</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6">
+        <v>-20.22222222222222</v>
+      </c>
+      <c r="L6" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +2171,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1916,37 +2182,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1954,37 +2220,37 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="K2">
         <v>4.888888888888889</v>
       </c>
       <c r="L2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1997,37 +2263,37 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K4">
         <v>-10.55555555555556</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2035,37 +2301,75 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="J5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="K5">
         <v>0.3333333333333333</v>
       </c>
       <c r="L5" t="s">
-        <v>96</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6">
+        <v>-4.555555555555555</v>
+      </c>
+      <c r="L6" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2075,7 +2379,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2086,37 +2390,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2124,37 +2428,37 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K2">
         <v>16.88888888888889</v>
       </c>
       <c r="L2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2167,28 +2471,28 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
         <v>37</v>
@@ -2197,7 +2501,7 @@
         <v>-10.66666666666667</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2205,37 +2509,45 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
         <v>118</v>
       </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" t="s">
-        <v>113</v>
-      </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="I5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K5">
         <v>5.666666666666667</v>
       </c>
       <c r="L5" t="s">
-        <v>95</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2245,7 +2557,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2256,37 +2568,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2294,37 +2606,37 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
         <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>16.33333333333333</v>
       </c>
       <c r="L2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2337,37 +2649,37 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I4" t="s">
         <v>49</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K4">
         <v>-13.11111111111111</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2375,37 +2687,45 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
         <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="J5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="K5">
         <v>7.444444444444445</v>
       </c>
       <c r="L5" t="s">
-        <v>95</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2415,7 +2735,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2426,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2480,6 +2800,11 @@
       </c>
       <c r="D5">
         <v>0.926440329218107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2489,7 +2814,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2500,13 +2825,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2554,6 +2879,11 @@
       </c>
       <c r="D5">
         <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>